<commit_message>
feat: Add first part of Viskosität protocol
</commit_message>
<xml_diff>
--- a/Physik/Praktikum/Versuch Viskosität/Ergebnisse.xlsx
+++ b/Physik/Praktikum/Versuch Viskosität/Ergebnisse.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/moritz/git/university/Physik/Praktikum/Versuch Viskosität/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B24AA5C-D57F-AC46-910D-1663A3053508}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12E136C4-054E-9343-82BD-BBA4E467D22D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{2E92C079-45FE-C74F-9508-FCE3F52F1DB7}"/>
+    <workbookView xWindow="4860" yWindow="21600" windowWidth="28800" windowHeight="18000" xr2:uid="{2E92C079-45FE-C74F-9508-FCE3F52F1DB7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="81">
   <si>
     <t>Messung 1</t>
   </si>
@@ -177,9 +177,6 @@
   </si>
   <si>
     <t>Erdanziehungskraft g [m/s^2]</t>
-  </si>
-  <si>
-    <t>Dichte von V2A-Stahl p_K [kg/m^3]</t>
   </si>
   <si>
     <t>Dichte von Getriebeöls OKS 3740 p_F [kg/m^3]</t>
@@ -371,37 +368,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-DE"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
@@ -1024,7 +991,7 @@
             <c:numRef>
               <c:f>Sheet1!$B$98:$C$98</c:f>
               <c:numCache>
-                <c:formatCode>#.##000000</c:formatCode>
+                <c:formatCode>#,##0.00000</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -1039,7 +1006,7 @@
             <c:numRef>
               <c:f>Sheet1!$B$99:$C$99</c:f>
               <c:numCache>
-                <c:formatCode>#.##000000</c:formatCode>
+                <c:formatCode>#,##0.00000</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>61.002957333333342</c:v>
@@ -1091,7 +1058,7 @@
             <c:numRef>
               <c:f>Sheet1!$E$98:$F$98</c:f>
               <c:numCache>
-                <c:formatCode>#.##000000</c:formatCode>
+                <c:formatCode>#,##0.00000</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -1106,7 +1073,7 @@
             <c:numRef>
               <c:f>Sheet1!$E$99:$F$99</c:f>
               <c:numCache>
-                <c:formatCode>#.##000000</c:formatCode>
+                <c:formatCode>#,##0.00000</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>124.35788849999999</c:v>
@@ -2829,8 +2796,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F361048E-DFA6-F64D-BD3E-240FE8B72108}">
   <dimension ref="A2:O102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="118" workbookViewId="0">
+      <selection activeCell="F57" sqref="F57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2991,7 +2958,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B11" s="1">
         <f>1/B6^2</f>
@@ -3437,7 +3404,7 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B45" s="1">
         <f>_xlfn.STDEV.S(B14:B23)</f>
@@ -3458,7 +3425,7 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B46" s="1">
         <f>B45/SQRT(10)</f>
@@ -3505,7 +3472,7 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B52" s="1">
         <v>0.01</v>
@@ -3513,7 +3480,7 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B53" s="1">
         <f>0.2*2</f>
@@ -3522,7 +3489,7 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B54" s="1">
         <v>5</v>
@@ -3530,7 +3497,7 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B56" s="1">
         <f>B54/B48</f>
@@ -3539,7 +3506,7 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B57" s="1">
         <f>(2*$B$52)/B6</f>
@@ -3560,7 +3527,7 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B58" s="1">
         <f>$B$53/B44</f>
@@ -3581,7 +3548,7 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B59" s="1">
         <f>($B$56+B57+B58)*B65</f>
@@ -3602,15 +3569,15 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B61" s="1">
         <v>860</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A62" s="1" t="s">
-        <v>47</v>
+      <c r="A62" s="1">
+        <v>0</v>
       </c>
       <c r="B62" s="1">
         <v>7900</v>
@@ -3626,7 +3593,7 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B65" s="1">
         <f>(($B$62-$B$61)*$B$63*B7^2*B44)/(18*$B$50)</f>
@@ -3645,12 +3612,12 @@
         <v>2.1842809805226677</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B66" s="1">
         <f>SUM(B65:E65)/4</f>
@@ -3659,7 +3626,7 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B68" s="1">
         <v>78.218999999999994</v>
@@ -3667,27 +3634,27 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B69" s="1">
         <f>(B68*(B62-B61)*B63)/(18*B50*1000^2)</f>
         <v>2.0007377280000003</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D71" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B74" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C74" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="C74" s="1" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.2">
@@ -3733,7 +3700,7 @@
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B79" s="1">
         <f>SUM(B76:B78)/3</f>
@@ -3746,7 +3713,7 @@
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B80" s="1">
         <f>_xlfn.STDEV.S(B76:B78)</f>
@@ -3759,7 +3726,7 @@
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B81" s="1">
         <f>B80/SQRT(3)</f>
@@ -3772,7 +3739,7 @@
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B82" s="1">
         <v>0.93410000000000004</v>
@@ -3783,7 +3750,7 @@
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B83" s="1">
         <v>2.0099999999999998</v>
@@ -3794,7 +3761,7 @@
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B85" s="1">
         <f>B82*B79</f>
@@ -3805,12 +3772,12 @@
         <v>124.35788849999999</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B87" s="1">
         <f>LOG(C79/B79)</f>
@@ -3819,7 +3786,7 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B88" s="1">
         <f>LOG((B83/2)/(C83/2))</f>
@@ -3828,19 +3795,19 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B89" s="1">
         <f>B87/B88</f>
         <v>6.3168243076087274</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B91" s="1">
         <v>0.87</v>
@@ -3851,7 +3818,7 @@
     </row>
     <row r="97" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B97" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C97" s="4"/>
       <c r="D97" s="4"/>
@@ -3892,7 +3859,7 @@
     </row>
     <row r="101" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B101" s="2">
         <v>10</v>
@@ -3939,7 +3906,7 @@
     </row>
     <row r="102" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B102" s="2">
         <v>1.02</v>

</xml_diff>

<commit_message>
feat: Finished protocol for Viskosität
</commit_message>
<xml_diff>
--- a/Physik/Praktikum/Versuch Viskosität/Ergebnisse.xlsx
+++ b/Physik/Praktikum/Versuch Viskosität/Ergebnisse.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/moritz/git/university/Physik/Praktikum/Versuch Viskosität/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12E136C4-054E-9343-82BD-BBA4E467D22D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A06B1D20-0F60-6B45-B441-B3E5E06AB949}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4860" yWindow="21600" windowWidth="28800" windowHeight="18000" xr2:uid="{2E92C079-45FE-C74F-9508-FCE3F52F1DB7}"/>
+    <workbookView xWindow="4860" yWindow="22100" windowWidth="28800" windowHeight="17500" xr2:uid="{2E92C079-45FE-C74F-9508-FCE3F52F1DB7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1138,6 +1138,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Gewichtskonzentration in %</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="#,##0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1215,6 +1270,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Kinematische</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> Viskosität in mm^2/s</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="#,##0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1264,6 +1379,37 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -2796,8 +2942,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F361048E-DFA6-F64D-BD3E-240FE8B72108}">
   <dimension ref="A2:O102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="118" workbookViewId="0">
-      <selection activeCell="F57" sqref="F57"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="108" workbookViewId="0">
+      <selection activeCell="Q118" sqref="Q118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
docs: Update Viskosität protocol
</commit_message>
<xml_diff>
--- a/Physik/Praktikum/Versuch Viskosität/Ergebnisse.xlsx
+++ b/Physik/Praktikum/Versuch Viskosität/Ergebnisse.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/moritz/git/university/Physik/Praktikum/Versuch Viskosität/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bwedu-my.sharepoint.com/personal/moritz_wieland_bwedu_de/Documents/Module/Physik/Praktikum/Versuch Viskosität/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A06B1D20-0F60-6B45-B441-B3E5E06AB949}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{A06B1D20-0F60-6B45-B441-B3E5E06AB949}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FA28D3DF-F5ED-194F-9964-073358E5C2E4}"/>
   <bookViews>
-    <workbookView xWindow="4860" yWindow="22100" windowWidth="28800" windowHeight="17500" xr2:uid="{2E92C079-45FE-C74F-9508-FCE3F52F1DB7}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{2E92C079-45FE-C74F-9508-FCE3F52F1DB7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1159,7 +1159,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-GB"/>
-                  <a:t>Gewichtskonzentration in %</a:t>
+                  <a:t>Gewichtskonzentration in Gew.-%</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -2942,8 +2942,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F361048E-DFA6-F64D-BD3E-240FE8B72108}">
   <dimension ref="A2:O102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="108" workbookViewId="0">
-      <selection activeCell="Q118" sqref="Q118"/>
+    <sheetView tabSelected="1" topLeftCell="A102" zoomScale="119" workbookViewId="0">
+      <selection activeCell="P135" sqref="P135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>